<commit_message>
Merge bulk upload template changes from cr0003
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2008389\Development\AdminPortal-latestCode\transparency-db-admin-portal\public\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\BEIS\source\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714F7CA4-6B4B-4BE6-8508-4C9348D4A27C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8614939B-09BC-409D-B6E7-05FA20477EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="12840" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -117,18 +117,12 @@
     <t>Tax measures (tax credit, or tax/duty exemption)</t>
   </si>
   <si>
-    <t>Large (more than 250 employees)</t>
-  </si>
-  <si>
     <t>South East</t>
   </si>
   <si>
     <t>Water supply; sewerage, waste management and remediation activities</t>
   </si>
   <si>
-    <t>Rescue aid</t>
-  </si>
-  <si>
     <t>Direct Grant</t>
   </si>
   <si>
@@ -163,20 +157,6 @@
   </si>
   <si>
     <t xml:space="preserve">From the Subsidy Scheme </t>
-  </si>
-  <si>
-    <t>Allowed values:
-1. Research and development
-2. Environmental protection 
-3. Energy efficiency 
-4. Culture/Heritage
-5. SME support 
-6. Regional development  
-7. Training 
-8. Employment
-9. Infrastructure 
-10. Rescue aid 
-11. Other</t>
   </si>
   <si>
     <t>If the User selects 'Other' in the Subsidy Objectives list then they can enter text describing their objective</t>
@@ -243,12 +223,6 @@
 2. Small organisation
 3. Medium organisation
 4. Large organisation</t>
-  </si>
-  <si>
-    <t>Micro – 0-9 employees
-Small – 10-49 employees
-Medium - 50-249 employees 
-Large – 250+ employees</t>
   </si>
   <si>
     <t>The name of the Granting Authority giving the award</t>
@@ -877,6 +851,32 @@
   </si>
   <si>
     <t>The selected file must be smaller than 500kb</t>
+  </si>
+  <si>
+    <t>Large (250 or more employees)</t>
+  </si>
+  <si>
+    <t>Rescue subsidy</t>
+  </si>
+  <si>
+    <t>Micro – 0-9 employees
+Small – 10-49 employees
+Medium - 50-249 employees 
+Large – 250 or more employees</t>
+  </si>
+  <si>
+    <t>Allowed values:
+1. Research and development
+2. Environmental protection 
+3. Energy efficiency 
+4. Culture/Heritage
+5. SME support 
+6. Regional development  
+7. Training 
+8. Employment
+9. Infrastructure 
+10. Rescue subsidy 
+11. Other</t>
   </si>
 </sst>
 </file>
@@ -1510,31 +1510,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1352"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="H1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A827" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="L837" sqref="L837"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="20" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="50.1796875" style="35" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="93" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37" style="35" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.7265625" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="72.453125" style="35" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="57.81640625" style="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.26953125" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.36328125" style="35" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="50.1796875" style="35" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.26953125" style="35" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.36328125" style="35" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.1796875" style="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="53.54296875" style="35" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="50.7265625" style="35" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="53.453125" style="35" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="50.6328125" style="35" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="80.1796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33.54296875" style="35" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.453125" style="35" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" style="35" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="33.81640625" style="35" customWidth="1"/>
-    <col min="17" max="17" width="108.7265625" style="35" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="108.6328125" style="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -11011,9 +11011,6 @@
       </c>
       <c r="F780" s="10"/>
       <c r="G780" s="23"/>
-      <c r="H780" s="35">
-        <v>2323132</v>
-      </c>
       <c r="I780" s="31"/>
       <c r="L780" s="31"/>
       <c r="O780" s="31"/>
@@ -11026,8 +11023,10 @@
       <c r="E781" s="26"/>
       <c r="F781" s="10"/>
       <c r="G781" s="23"/>
+      <c r="H781" s="35">
+        <v>2323132</v>
+      </c>
       <c r="I781" s="31"/>
-      <c r="L781" s="31"/>
       <c r="O781" s="31"/>
       <c r="P781" s="26"/>
       <c r="Q781" s="34"/>
@@ -13760,8 +13759,12 @@
       <c r="D1352" s="26"/>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 Public</oddFooter>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
@@ -13830,7 +13833,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13838,22 +13841,22 @@
     <col min="1" max="1" width="57" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.453125" customWidth="1"/>
     <col min="3" max="3" width="130.81640625" customWidth="1"/>
-    <col min="4" max="4" width="69.7265625" customWidth="1"/>
+    <col min="4" max="4" width="69.6328125" customWidth="1"/>
     <col min="5" max="16384" width="12.1796875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>36</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -13862,16 +13865,16 @@
     </row>
     <row r="2" spans="1:8" ht="20" x14ac:dyDescent="0.35">
       <c r="A2" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="D2" s="37" t="s">
         <v>38</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>40</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -13883,10 +13886,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D3" s="37"/>
       <c r="E3" s="2"/>
@@ -13899,10 +13902,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>42</v>
+        <v>178</v>
       </c>
       <c r="D4" s="37"/>
       <c r="E4" s="2"/>
@@ -13916,7 +13919,7 @@
       </c>
       <c r="B5" s="37"/>
       <c r="C5" s="39" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="2"/>
@@ -13929,10 +13932,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="2"/>
@@ -13946,7 +13949,7 @@
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="37" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="2"/>
@@ -13959,13 +13962,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -13974,13 +13977,13 @@
     </row>
     <row r="9" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="37" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="2"/>
@@ -13993,10 +13996,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="2"/>
@@ -14009,10 +14012,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="2"/>
@@ -14025,10 +14028,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="2"/>
@@ -14041,13 +14044,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>56</v>
+        <v>177</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -14059,10 +14062,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="2"/>
@@ -14075,13 +14078,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -14090,16 +14093,16 @@
     </row>
     <row r="16" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="38" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -14111,10 +14114,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D17" s="37"/>
       <c r="E17" s="2"/>
@@ -14124,13 +14127,13 @@
     </row>
     <row r="18" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A18" s="39" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D18" s="39"/>
     </row>
@@ -14138,6 +14141,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 Public</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -14145,22 +14151,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.1796875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="78.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.36328125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="81.453125" style="4" customWidth="1"/>
     <col min="7" max="7" width="108" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="46.453125" style="4" customWidth="1"/>
     <col min="9" max="10" width="9.1796875" style="4"/>
-    <col min="11" max="11" width="47.26953125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.36328125" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
@@ -14169,16 +14175,16 @@
         <v>15</v>
       </c>
       <c r="B1" s="45" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E1" s="45" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>2</v>
@@ -14187,95 +14193,95 @@
         <v>16</v>
       </c>
       <c r="H1" s="45" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H2" s="46" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H3" s="46" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4" s="46" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>26</v>
+        <v>175</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>18</v>
@@ -14285,77 +14291,77 @@
         <v>24</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="47"/>
       <c r="D6" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H6" s="46" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H7" s="46" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H8" s="46" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -14364,61 +14370,61 @@
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13" t="s">
-        <v>29</v>
+        <v>176</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H9" s="46" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H12" s="13"/>
     </row>
@@ -14431,10 +14437,10 @@
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H13" s="13"/>
     </row>
@@ -14446,7 +14452,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H14" s="13"/>
     </row>
@@ -14458,7 +14464,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H15" s="13"/>
     </row>
@@ -14470,7 +14476,7 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H16" s="13"/>
     </row>
@@ -14482,7 +14488,7 @@
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H17" s="13"/>
     </row>
@@ -14506,7 +14512,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H19" s="13"/>
     </row>
@@ -14518,7 +14524,7 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H20" s="13"/>
     </row>
@@ -14530,7 +14536,7 @@
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H21" s="13"/>
     </row>
@@ -14542,7 +14548,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H22" s="13"/>
     </row>
@@ -14555,6 +14561,9 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 Public</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -14566,40 +14575,40 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.453125" customWidth="1"/>
-    <col min="4" max="4" width="74.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="74.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="51" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14607,7 +14616,7 @@
       <c r="B3" s="52"/>
       <c r="C3" s="52"/>
       <c r="D3" s="39" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14615,7 +14624,7 @@
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="39" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14623,7 +14632,7 @@
       <c r="B5" s="53"/>
       <c r="C5" s="53"/>
       <c r="D5" s="39" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -14631,13 +14640,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14645,7 +14654,7 @@
       <c r="B7" s="49"/>
       <c r="C7" s="49"/>
       <c r="D7" s="15" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14653,7 +14662,7 @@
       <c r="B8" s="49"/>
       <c r="C8" s="49"/>
       <c r="D8" s="39" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14661,7 +14670,7 @@
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
       <c r="D9" s="39" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="240" x14ac:dyDescent="0.35">
@@ -14669,11 +14678,11 @@
         <v>2</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="15" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.45">
@@ -14681,13 +14690,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D11" s="39" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E11" s="18"/>
     </row>
@@ -14696,11 +14705,11 @@
         <v>4</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -14709,10 +14718,10 @@
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="41" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="100" x14ac:dyDescent="0.35">
@@ -14720,27 +14729,27 @@
         <v>6</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="129" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C15" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="37" t="s">
         <v>146</v>
-      </c>
-      <c r="D15" s="37" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14748,11 +14757,11 @@
         <v>8</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -14760,13 +14769,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="48" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14774,7 +14783,7 @@
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
       <c r="D18" s="43" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14782,7 +14791,7 @@
       <c r="B19" s="49"/>
       <c r="C19" s="49"/>
       <c r="D19" s="43" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14790,7 +14799,7 @@
       <c r="B20" s="49"/>
       <c r="C20" s="49"/>
       <c r="D20" s="43" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14798,7 +14807,7 @@
       <c r="B21" s="50"/>
       <c r="C21" s="50"/>
       <c r="D21" s="39" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14806,25 +14815,25 @@
         <v>10</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="117" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="40" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C23" s="39"/>
       <c r="D23" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="236.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -14832,13 +14841,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14846,23 +14855,23 @@
         <v>13</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C25" s="39"/>
       <c r="D25" s="37" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="40" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C26" s="39"/>
       <c r="D26" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.35">
@@ -14870,28 +14879,28 @@
         <v>15</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C27" s="39"/>
       <c r="D27" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="400" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="39" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="20" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="20"/>
@@ -14899,7 +14908,7 @@
     </row>
     <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="20"/>
@@ -14907,7 +14916,7 @@
     </row>
     <row r="31" spans="1:4" ht="20" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="20"/>
@@ -14915,7 +14924,7 @@
     </row>
     <row r="32" spans="1:4" ht="40" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="20"/>
@@ -14923,7 +14932,7 @@
     </row>
     <row r="33" spans="1:4" ht="40" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="20"/>
@@ -14931,7 +14940,7 @@
     </row>
     <row r="34" spans="1:4" ht="40" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="20"/>
@@ -14939,7 +14948,7 @@
     </row>
     <row r="35" spans="1:4" ht="40" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="20"/>
@@ -14959,6 +14968,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 Public</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -15483,4 +15495,10 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="2" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
refactor: reverting changes to fix merge conflict issues
AB#204
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/billbatten/Projects/Subsidy/transparency-db-admin-portal/public/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B346D9F7-1E07-1C45-BB80-4469904EE6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C3D849-F881-8248-8724-85E552700FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="179">
   <si>
     <t>Subsidy Control (SC) Number</t>
   </si>
@@ -177,9 +177,6 @@
   </si>
   <si>
     <t>Mandatory when a Tax Measure</t>
-  </si>
-  <si>
-    <t>Where the Full Amount is a Tax Measure enter as a Range.</t>
   </si>
   <si>
     <t xml:space="preserve"> 1- 60000
@@ -291,9 +288,6 @@
     <t>Subsidy instrument</t>
   </si>
   <si>
-    <t>Amount Range</t>
-  </si>
-  <si>
     <t>East Midlands</t>
   </si>
   <si>
@@ -306,9 +300,6 @@
     <t>Culture or Heritage</t>
   </si>
   <si>
-    <t>1- 60000</t>
-  </si>
-  <si>
     <t>East of England</t>
   </si>
   <si>
@@ -324,9 +315,6 @@
     <t>Activities of extraterritorial organisations and bodies</t>
   </si>
   <si>
-    <t>60001-500000</t>
-  </si>
-  <si>
     <t>London</t>
   </si>
   <si>
@@ -342,9 +330,6 @@
     <t>Energy efficiency</t>
   </si>
   <si>
-    <t>500001-1000000</t>
-  </si>
-  <si>
     <t>North East</t>
   </si>
   <si>
@@ -354,9 +339,6 @@
     <t>Administrative and support service activities</t>
   </si>
   <si>
-    <t>1000001-2000000</t>
-  </si>
-  <si>
     <t>North West</t>
   </si>
   <si>
@@ -369,9 +351,6 @@
     <t>Agriculture, forestry and fishing</t>
   </si>
   <si>
-    <t>2000001-5000000</t>
-  </si>
-  <si>
     <t>Northern Ireland</t>
   </si>
   <si>
@@ -381,9 +360,6 @@
     <t>Arts, entertainment and recreation</t>
   </si>
   <si>
-    <t>5000001-10000000</t>
-  </si>
-  <si>
     <t>Scotland</t>
   </si>
   <si>
@@ -393,15 +369,9 @@
     <t>Construction</t>
   </si>
   <si>
-    <t>10000001-30000000</t>
-  </si>
-  <si>
     <t>Education</t>
   </si>
   <si>
-    <t>30000001  or more</t>
-  </si>
-  <si>
     <t>South West</t>
   </si>
   <si>
@@ -409,9 +379,6 @@
   </si>
   <si>
     <t>Electricity, gas, steam and air conditioning supply</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
   <si>
     <t>Wales</t>
@@ -886,6 +853,9 @@
     <t>Standalone Award</t>
   </si>
   <si>
+    <t>Subsidy Description</t>
+  </si>
+  <si>
     <t>Yes/No</t>
   </si>
   <si>
@@ -897,6 +867,9 @@
   <si>
     <t>Yes
 No</t>
+  </si>
+  <si>
+    <t>This decription should include TCA requirements such as relevant time limits or other conditions attached to the scheme.</t>
   </si>
   <si>
     <t>Limit 2000 characters</t>
@@ -907,13 +880,7 @@
 </t>
   </si>
   <si>
-    <t>Subsidy Award Description</t>
-  </si>
-  <si>
-    <t>Optional</t>
-  </si>
-  <si>
-    <t>This description should include TCA requirements such as relevant time limits or other conditions attached to the scheme.</t>
+    <t>Where the Full Amount is a Tax Measure enter as a Range in the format shown on the next column. Two numbers seperated by a ' - '.</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1254,6 +1221,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1560,7 +1528,7 @@
     <sheetView zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1594,10 +1562,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>2</v>
@@ -1645,7 +1613,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="23"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -1654,7 +1622,7 @@
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="23"/>
+      <c r="I2" s="54"/>
       <c r="J2" s="25"/>
       <c r="K2" s="11"/>
       <c r="L2" s="26"/>
@@ -1666,7 +1634,7 @@
       <c r="R2" s="10"/>
       <c r="S2" s="34"/>
     </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
@@ -1675,7 +1643,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
-      <c r="I3" s="28"/>
+      <c r="I3" s="54"/>
       <c r="J3" s="25"/>
       <c r="K3" s="23"/>
       <c r="L3" s="28"/>
@@ -11098,9 +11066,6 @@
       <c r="G781" s="26"/>
       <c r="H781" s="10"/>
       <c r="I781" s="23"/>
-      <c r="J781" s="35">
-        <v>2323132</v>
-      </c>
       <c r="K781" s="31"/>
       <c r="Q781" s="31"/>
       <c r="R781" s="26"/>
@@ -13842,7 +13807,7 @@
   </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Dropdown!$G$2:$G$22</xm:f>
@@ -13885,12 +13850,6 @@
           </x14:formula1>
           <xm:sqref>R2:R836</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000007000000}">
-          <x14:formula1>
-            <xm:f>Dropdown!$H$2:$H$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I836</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
           <x14:formula1>
             <xm:f>Dropdown!$F$2:$F$13</xm:f>
@@ -13899,7 +13858,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E0952469-FEE6-48C2-A15D-910C0C2B113B}">
           <x14:formula1>
-            <xm:f>Dropdown!$I$2:$I$3</xm:f>
+            <xm:f>Dropdown!$H$2:$H$3</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C837</xm:sqref>
         </x14:dataValidation>
@@ -13914,7 +13873,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13980,16 +13939,16 @@
     </row>
     <row r="4" spans="1:8" ht="126" x14ac:dyDescent="0.2">
       <c r="A4" s="38" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -13998,16 +13957,14 @@
     </row>
     <row r="5" spans="1:8" ht="42" x14ac:dyDescent="0.2">
       <c r="A5" s="38" t="s">
-        <v>187</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>188</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="B5" s="37"/>
       <c r="C5" s="37" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -14022,7 +13979,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="2"/>
@@ -14082,10 +14039,10 @@
         <v>43</v>
       </c>
       <c r="C10" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="37" t="s">
         <v>44</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>45</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -14094,13 +14051,13 @@
     </row>
     <row r="11" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="C11" s="37" t="s">
         <v>47</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>48</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="2"/>
@@ -14116,7 +14073,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="2"/>
@@ -14132,7 +14089,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="37"/>
       <c r="E13" s="2"/>
@@ -14148,7 +14105,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="2"/>
@@ -14164,10 +14121,10 @@
         <v>36</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -14182,7 +14139,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="37"/>
       <c r="E16" s="2"/>
@@ -14198,10 +14155,10 @@
         <v>36</v>
       </c>
       <c r="C17" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="37" t="s">
         <v>54</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>55</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -14210,16 +14167,16 @@
     </row>
     <row r="18" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="37" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -14234,7 +14191,7 @@
         <v>36</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D19" s="37"/>
       <c r="E19" s="2"/>
@@ -14244,13 +14201,13 @@
     </row>
     <row r="20" spans="1:8" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A20" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="37" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="39"/>
     </row>
@@ -14266,9 +14223,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
+    <sheetView topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14285,21 +14244,21 @@
     <col min="12" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="45" t="s">
-        <v>63</v>
-      </c>
       <c r="E1" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" s="45" t="s">
         <v>2</v>
@@ -14308,18 +14267,15 @@
         <v>16</v>
       </c>
       <c r="H1" s="45" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>64</v>
-      </c>
-      <c r="I1" s="45" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>66</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>20</v>
@@ -14328,87 +14284,78 @@
         <v>28</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>29</v>
       </c>
       <c r="H2" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="I2" s="46" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="44" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="C4" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="D4" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="I3" s="46" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="44" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="E4" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="I4" s="46"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+      <c r="H4" s="46"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>18</v>
@@ -14418,79 +14365,67 @@
         <v>24</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="I5" s="46"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="H5" s="46"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="47"/>
       <c r="D6" s="13" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="H6" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="46"/>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="H6" s="46"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="46"/>
+    </row>
+    <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
         <v>87</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="H7" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="I7" s="46"/>
-    </row>
-    <row r="8" spans="1:10" ht="21" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>95</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="H8" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="I8" s="46"/>
-    </row>
-    <row r="9" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+      <c r="H8" s="46"/>
+    </row>
+    <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>26</v>
       </c>
@@ -14501,68 +14436,61 @@
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="H9" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="I9" s="46"/>
-    </row>
-    <row r="10" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="H9" s="46"/>
+    </row>
+    <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>22</v>
       </c>
@@ -14571,15 +14499,14 @@
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -14587,12 +14514,11 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -14600,12 +14526,11 @@
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-    </row>
-    <row r="16" spans="1:10" ht="21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="13"/>
@@ -14613,12 +14538,11 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-    </row>
-    <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.2">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -14626,12 +14550,11 @@
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-    </row>
-    <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
@@ -14642,9 +14565,8 @@
         <v>23</v>
       </c>
       <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.2">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -14652,12 +14574,11 @@
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-    </row>
-    <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -14665,12 +14586,11 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.2">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -14681,9 +14601,8 @@
         <v>27</v>
       </c>
       <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="1:9" ht="21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.2">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -14691,20 +14610,19 @@
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="13" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A13">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="G14:H22">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="H14:H22">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I14:I22">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="G14:G22">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -14732,16 +14650,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14749,13 +14667,13 @@
         <v>35</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14763,7 +14681,7 @@
       <c r="B3" s="52"/>
       <c r="C3" s="52"/>
       <c r="D3" s="39" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14771,7 +14689,7 @@
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="39" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14779,7 +14697,7 @@
       <c r="B5" s="53"/>
       <c r="C5" s="53"/>
       <c r="D5" s="39" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14787,13 +14705,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -14801,7 +14719,7 @@
       <c r="B7" s="49"/>
       <c r="C7" s="49"/>
       <c r="D7" s="15" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -14809,7 +14727,7 @@
       <c r="B8" s="49"/>
       <c r="C8" s="49"/>
       <c r="D8" s="39" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -14817,7 +14735,7 @@
       <c r="B9" s="50"/>
       <c r="C9" s="50"/>
       <c r="D9" s="39" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="252" x14ac:dyDescent="0.2">
@@ -14825,11 +14743,11 @@
         <v>2</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="15" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -14837,10 +14755,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D11" s="39" t="s">
         <v>40</v>
@@ -14852,11 +14770,11 @@
         <v>4</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14865,10 +14783,10 @@
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="41" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.2">
@@ -14876,27 +14794,27 @@
         <v>6</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="129" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14904,11 +14822,11 @@
         <v>8</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14916,13 +14834,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="48" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14930,7 +14848,7 @@
       <c r="B18" s="49"/>
       <c r="C18" s="49"/>
       <c r="D18" s="43" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14938,7 +14856,7 @@
       <c r="B19" s="49"/>
       <c r="C19" s="49"/>
       <c r="D19" s="43" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14946,7 +14864,7 @@
       <c r="B20" s="49"/>
       <c r="C20" s="49"/>
       <c r="D20" s="43" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14954,7 +14872,7 @@
       <c r="B21" s="50"/>
       <c r="C21" s="50"/>
       <c r="D21" s="39" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -14962,25 +14880,25 @@
         <v>10</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="40" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C23" s="39"/>
       <c r="D23" s="15" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="236.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14988,13 +14906,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="154.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -15002,23 +14920,23 @@
         <v>13</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C25" s="39"/>
       <c r="D25" s="37" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="40" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C26" s="39"/>
       <c r="D26" s="15" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.2">
@@ -15026,28 +14944,28 @@
         <v>15</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C27" s="39"/>
       <c r="D27" s="15" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="400" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="15" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B29" s="19"/>
       <c r="C29" s="20"/>
@@ -15055,7 +14973,7 @@
     </row>
     <row r="30" spans="1:4" ht="63" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B30" s="19"/>
       <c r="C30" s="20"/>
@@ -15063,7 +14981,7 @@
     </row>
     <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="B31" s="19"/>
       <c r="C31" s="20"/>
@@ -15071,7 +14989,7 @@
     </row>
     <row r="32" spans="1:4" ht="42" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B32" s="19"/>
       <c r="C32" s="20"/>
@@ -15079,7 +14997,7 @@
     </row>
     <row r="33" spans="1:4" ht="42" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="B33" s="19"/>
       <c r="C33" s="20"/>
@@ -15087,7 +15005,7 @@
     </row>
     <row r="34" spans="1:4" ht="42" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="20"/>
@@ -15095,7 +15013,7 @@
     </row>
     <row r="35" spans="1:4" ht="42" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="20"/>
@@ -15122,42 +15040,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15525,87 +15466,59 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15628,18 +15541,23 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
refactor: Updated bulk award upload template wording
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.robinson\Documents\BEIS\transparency-db-admin-portal\public\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan.Humphreys\Documents\BEIS STS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4DF061-86D2-4168-9673-9B4124E57E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD15E8F3-6028-40D6-87CE-51BE5E787C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="185">
   <si>
     <t>Subsidy Control (SC) Number</t>
   </si>
@@ -894,6 +894,12 @@
 Charity Number can have up to 8 numbers
 VAT Number are nine digits long.
 UTR Number is 10 digits long</t>
+  </si>
+  <si>
+    <t>Subsidy Form</t>
+  </si>
+  <si>
+    <t>Subsidy Form "Other" - Text</t>
   </si>
 </sst>
 </file>
@@ -1507,10 +1513,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1352"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
@@ -1560,10 +1566,10 @@
         <v>3</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>4</v>
+        <v>183</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>5</v>
+        <v>184</v>
       </c>
       <c r="J1" s="20" t="s">
         <v>6</v>
@@ -13869,7 +13875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -15053,55 +15059,50 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15469,60 +15470,86 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15545,31 +15572,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
chore: updated award bulk upload template
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.robinson\Documents\BEIS\transparency-db-admin-portal\public\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan.Humphreys\Documents\BEIS STS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4DF061-86D2-4168-9673-9B4124E57E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83621565-FACC-4F17-A7E6-14BE80E13EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="185">
   <si>
     <t>Subsidy Control (SC) Number</t>
   </si>
@@ -171,9 +171,6 @@
 6. Provision of goods or services below market prices 
 7. Purchase of goods or services above market prices
 8. Other</t>
-  </si>
-  <si>
-    <t>If the User selects 'Other' in the Subsidy Instrument list then they can enter text describing their Instrument</t>
   </si>
   <si>
     <t>Mandatory when a Tax Measure</t>
@@ -894,6 +891,15 @@
 Charity Number can have up to 8 numbers
 VAT Number are nine digits long.
 UTR Number is 10 digits long</t>
+  </si>
+  <si>
+    <t>Subsidy Form</t>
+  </si>
+  <si>
+    <t>Subsidy Form "Other" - Text</t>
+  </si>
+  <si>
+    <t>If the User selects 'Other' in the Subsidy Form list then they can enter text describing their form</t>
   </si>
 </sst>
 </file>
@@ -1507,10 +1513,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1352"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
@@ -1545,13 +1551,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D1" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>167</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>168</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>2</v>
@@ -1560,10 +1566,10 @@
         <v>3</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>4</v>
+        <v>182</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>5</v>
+        <v>183</v>
       </c>
       <c r="J1" s="20" t="s">
         <v>6</v>
@@ -1584,7 +1590,7 @@
         <v>11</v>
       </c>
       <c r="P1" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q1" s="20" t="s">
         <v>13</v>
@@ -13869,8 +13875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A6" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13935,14 +13941,14 @@
     </row>
     <row r="4" spans="1:8" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -13951,16 +13957,16 @@
     </row>
     <row r="5" spans="1:8" ht="142.80000000000001" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -13969,14 +13975,14 @@
     </row>
     <row r="6" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -13991,7 +13997,7 @@
         <v>36</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="2"/>
@@ -14015,7 +14021,7 @@
     </row>
     <row r="9" spans="1:8" ht="183.6" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
-        <v>4</v>
+        <v>182</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>36</v>
@@ -14031,11 +14037,11 @@
     </row>
     <row r="10" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
-        <v>5</v>
+        <v>183</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="29" t="s">
-        <v>42</v>
+        <v>184</v>
       </c>
       <c r="D10" s="29"/>
       <c r="E10" s="2"/>
@@ -14048,13 +14054,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="D11" s="29" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>44</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -14063,13 +14069,13 @@
     </row>
     <row r="12" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="C12" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>47</v>
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="2"/>
@@ -14085,7 +14091,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="2"/>
@@ -14101,7 +14107,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="2"/>
@@ -14117,7 +14123,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="2"/>
@@ -14133,10 +14139,10 @@
         <v>36</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -14145,13 +14151,13 @@
     </row>
     <row r="17" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B17" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D17" s="29"/>
       <c r="E17" s="2"/>
@@ -14167,10 +14173,10 @@
         <v>36</v>
       </c>
       <c r="C18" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="29" t="s">
         <v>51</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>52</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -14179,16 +14185,16 @@
     </row>
     <row r="19" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -14203,7 +14209,7 @@
         <v>36</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="2"/>
@@ -14213,13 +14219,13 @@
     </row>
     <row r="21" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A21" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="30"/>
     </row>
@@ -14261,16 +14267,16 @@
         <v>15</v>
       </c>
       <c r="B1" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="D1" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>60</v>
-      </c>
       <c r="E1" s="34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1" s="34" t="s">
         <v>2</v>
@@ -14279,15 +14285,15 @@
         <v>16</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>62</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>20</v>
@@ -14296,62 +14302,62 @@
         <v>28</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>63</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>64</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>29</v>
       </c>
       <c r="H2" s="35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>69</v>
-      </c>
       <c r="H3" s="35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C4" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="D4" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="E4" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>74</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>30</v>
@@ -14361,13 +14367,13 @@
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>76</v>
-      </c>
       <c r="C5" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>18</v>
@@ -14377,63 +14383,63 @@
         <v>24</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" s="35"/>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="36"/>
       <c r="D6" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>80</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>81</v>
       </c>
       <c r="H6" s="35"/>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H8" s="35"/>
     </row>
@@ -14448,57 +14454,57 @@
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>91</v>
       </c>
       <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>93</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>96</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>97</v>
       </c>
       <c r="H12" s="12"/>
     </row>
@@ -14511,10 +14517,10 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>98</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>99</v>
       </c>
       <c r="H13" s="12"/>
     </row>
@@ -14526,7 +14532,7 @@
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H14" s="12"/>
     </row>
@@ -14538,7 +14544,7 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H15" s="12"/>
     </row>
@@ -14550,7 +14556,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H16" s="12"/>
     </row>
@@ -14562,7 +14568,7 @@
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" s="12"/>
     </row>
@@ -14586,7 +14592,7 @@
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H19" s="12"/>
     </row>
@@ -14598,7 +14604,7 @@
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H20" s="12"/>
     </row>
@@ -14622,7 +14628,7 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H22" s="12"/>
     </row>
@@ -14662,16 +14668,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>109</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -14679,13 +14685,13 @@
         <v>35</v>
       </c>
       <c r="B2" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="D2" s="30" t="s">
         <v>112</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14693,7 +14699,7 @@
       <c r="B3" s="42"/>
       <c r="C3" s="42"/>
       <c r="D3" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14701,7 +14707,7 @@
       <c r="B4" s="42"/>
       <c r="C4" s="42"/>
       <c r="D4" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14709,7 +14715,7 @@
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -14717,13 +14723,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="D6" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -14731,7 +14737,7 @@
       <c r="B7" s="39"/>
       <c r="C7" s="39"/>
       <c r="D7" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -14739,7 +14745,7 @@
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
       <c r="D8" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -14747,7 +14753,7 @@
       <c r="B9" s="40"/>
       <c r="C9" s="40"/>
       <c r="D9" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="245.4" x14ac:dyDescent="0.3">
@@ -14755,11 +14761,11 @@
         <v>2</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C10" s="30"/>
       <c r="D10" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.4">
@@ -14767,10 +14773,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="30" t="s">
         <v>122</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>123</v>
       </c>
       <c r="D11" s="30" t="s">
         <v>40</v>
@@ -14782,11 +14788,11 @@
         <v>4</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" s="30"/>
       <c r="D12" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -14795,10 +14801,10 @@
       </c>
       <c r="B13" s="31"/>
       <c r="C13" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="123" x14ac:dyDescent="0.3">
@@ -14806,27 +14812,27 @@
         <v>6</v>
       </c>
       <c r="B14" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="D14" s="29" t="s">
         <v>128</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="129" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="C15" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="29" t="s">
         <v>131</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14834,11 +14840,11 @@
         <v>8</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -14846,13 +14852,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="D17" s="14" t="s">
         <v>136</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14860,7 +14866,7 @@
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
       <c r="D18" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14868,7 +14874,7 @@
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
       <c r="D19" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14876,7 +14882,7 @@
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
       <c r="D20" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14884,7 +14890,7 @@
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
       <c r="D21" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14892,25 +14898,25 @@
         <v>10</v>
       </c>
       <c r="B22" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="D22" s="14" t="s">
         <v>142</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" s="31" t="s">
         <v>144</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>145</v>
       </c>
       <c r="C23" s="30"/>
       <c r="D23" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="236.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -14918,13 +14924,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>146</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="154.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -14932,23 +14938,23 @@
         <v>13</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="31" t="s">
         <v>150</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>151</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.3">
@@ -14956,28 +14962,28 @@
         <v>15</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="400.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="19"/>
@@ -14985,7 +14991,7 @@
     </row>
     <row r="30" spans="1:4" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" s="18"/>
       <c r="C30" s="19"/>
@@ -14993,7 +14999,7 @@
     </row>
     <row r="31" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B31" s="18"/>
       <c r="C31" s="19"/>
@@ -15001,7 +15007,7 @@
     </row>
     <row r="32" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B32" s="18"/>
       <c r="C32" s="19"/>
@@ -15009,7 +15015,7 @@
     </row>
     <row r="33" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B33" s="18"/>
       <c r="C33" s="19"/>
@@ -15017,7 +15023,7 @@
     </row>
     <row r="34" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -15025,7 +15031,7 @@
     </row>
     <row r="35" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="19"/>

</xml_diff>

<commit_message>
style: moved policy URL fields to below description - reordered bulk upload template to reflect this
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan.Humphreys\Documents\BEIS STS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D231B1A-315B-4B31-A3EB-45E2F6102F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A022C194-DCC5-4EB1-90E3-CF41C691B6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5304" yWindow="2640" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -1580,10 +1580,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1352"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
@@ -1592,9 +1592,9 @@
     <col min="2" max="2" width="93" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.21875" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.77734375" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="93" style="23" customWidth="1"/>
+    <col min="5" max="5" width="93" style="23" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61" style="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" style="23" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="54.6640625" style="23" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="72.44140625" style="23" bestFit="1" customWidth="1"/>
@@ -1625,14 +1625,14 @@
       <c r="D1" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="G1" s="39" t="s">
         <v>183</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>167</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>2</v>
@@ -1709,9 +1709,9 @@
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
-      <c r="E3" s="10"/>
+      <c r="E3" s="26"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="26"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="24"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -1733,9 +1733,9 @@
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
-      <c r="E4" s="10"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="26"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="24"/>
       <c r="I4" s="9"/>
       <c r="J4" s="24"/>
@@ -13901,11 +13901,11 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1000" xr:uid="{D615B357-0729-431F-894C-730DD8C55F63}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G1000" xr:uid="{D615B357-0729-431F-894C-730DD8C55F63}">
       <formula1>0</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1000" xr:uid="{0EAC9FAD-095F-4C8A-9100-058828F1537D}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1000" xr:uid="{0EAC9FAD-095F-4C8A-9100-058828F1537D}">
       <formula1>0</formula1>
       <formula2>255</formula2>
     </dataValidation>
@@ -13982,7 +13982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -15201,101 +15201,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15663,44 +15568,102 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15723,6 +15686,43 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
chore: updated template in line with AB#170
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan.Humphreys\Documents\BEIS STS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D231B1A-315B-4B31-A3EB-45E2F6102F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC58772C-AAAF-494E-8B51-0F0C86AA08E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1583,7 +1583,7 @@
     <sheetView topLeftCell="B1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
@@ -1592,9 +1592,9 @@
     <col min="2" max="2" width="93" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.21875" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.77734375" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="93" style="23" customWidth="1"/>
+    <col min="5" max="5" width="93" style="23" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61" style="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37" style="23" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="54.6640625" style="23" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="72.44140625" style="23" bestFit="1" customWidth="1"/>
@@ -1625,14 +1625,14 @@
       <c r="D1" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="G1" s="39" t="s">
         <v>183</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>167</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>2</v>
@@ -1709,9 +1709,9 @@
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
       <c r="D3" s="26"/>
-      <c r="E3" s="10"/>
+      <c r="E3" s="26"/>
       <c r="F3" s="10"/>
-      <c r="G3" s="26"/>
+      <c r="G3" s="10"/>
       <c r="H3" s="24"/>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
@@ -1733,9 +1733,9 @@
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
-      <c r="E4" s="10"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="10"/>
-      <c r="G4" s="26"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="24"/>
       <c r="I4" s="9"/>
       <c r="J4" s="24"/>
@@ -13901,11 +13901,11 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1000" xr:uid="{D615B357-0729-431F-894C-730DD8C55F63}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G1000" xr:uid="{D615B357-0729-431F-894C-730DD8C55F63}">
       <formula1>0</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1000" xr:uid="{0EAC9FAD-095F-4C8A-9100-058828F1537D}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1000" xr:uid="{0EAC9FAD-095F-4C8A-9100-058828F1537D}">
       <formula1>0</formula1>
       <formula2>255</formula2>
     </dataValidation>
@@ -14080,52 +14080,52 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="82.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>192</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="B6" s="29"/>
       <c r="C6" s="29" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="61.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="82.2" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>192</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="61.8" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" s="29"/>
+        <v>189</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>192</v>
+      </c>
       <c r="C8" s="29" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>

</xml_diff>

<commit_message>
chore: reordered help sheet ordering to reflect frontend
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan.Humphreys\Documents\BEIS STS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A022C194-DCC5-4EB1-90E3-CF41C691B6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC58772C-AAAF-494E-8B51-0F0C86AA08E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5304" yWindow="2640" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -1580,7 +1580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
       <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
@@ -13982,7 +13982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -14080,52 +14080,52 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="82.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>192</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="B6" s="29"/>
       <c r="C6" s="29" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="61.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="82.2" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>192</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="61.8" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
-        <v>167</v>
-      </c>
-      <c r="B8" s="29"/>
+        <v>189</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>192</v>
+      </c>
       <c r="C8" s="29" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>180</v>
+        <v>191</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -15201,6 +15201,101 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15568,102 +15663,44 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15686,43 +15723,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
updated the bulk upload templates to hide dropdown tabs
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bill.batten\Documents\Projects\STS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96803ABA-2B37-4720-8DD5-9576EF2D69D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C62889-C1DF-4FBA-86E1-B5BB5986D4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
     <sheet name="Help &amp; Guidance" sheetId="2" r:id="rId2"/>
-    <sheet name="Dropdown" sheetId="3" r:id="rId3"/>
+    <sheet name="Dropdown" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="Rules" sheetId="5" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
@@ -1284,6 +1284,21 @@
     <xf numFmtId="49" fontId="13" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1301,21 +1316,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14455,7 +14455,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -14525,7 +14525,7 @@
       <c r="G2" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="44" t="s">
+      <c r="H2" s="38" t="s">
         <v>169</v>
       </c>
       <c r="I2" s="33" t="s">
@@ -14554,7 +14554,7 @@
       <c r="G3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="H3" s="38" t="s">
         <v>170</v>
       </c>
       <c r="I3" s="33" t="s">
@@ -14583,7 +14583,7 @@
       <c r="G4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="44"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="33" t="s">
         <v>199</v>
       </c>
@@ -14608,8 +14608,8 @@
       <c r="G5" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="46"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="40"/>
     </row>
     <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -14627,8 +14627,8 @@
       <c r="G6" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="H6" s="44"/>
-      <c r="I6" s="47"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="41"/>
     </row>
     <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -14646,8 +14646,8 @@
       <c r="G7" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="48"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="42"/>
     </row>
     <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -14665,8 +14665,8 @@
       <c r="G8" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="44"/>
-      <c r="I8" s="48"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
@@ -14684,8 +14684,8 @@
       <c r="G9" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H9" s="44"/>
-      <c r="I9" s="48"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
@@ -14701,8 +14701,8 @@
       <c r="G10" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="H10" s="45"/>
-      <c r="I10" s="48"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="42"/>
     </row>
     <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
@@ -14718,7 +14718,7 @@
       <c r="G11" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="I11" s="48"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
@@ -14734,8 +14734,8 @@
       <c r="G12" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="H12" s="45"/>
-      <c r="I12" s="48"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="42"/>
     </row>
     <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
@@ -14751,8 +14751,8 @@
       <c r="G13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="H13" s="45"/>
-      <c r="I13" s="48"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="42"/>
     </row>
     <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
@@ -14764,8 +14764,8 @@
       <c r="G14" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="H14" s="45"/>
-      <c r="I14" s="48"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="42"/>
     </row>
     <row r="15" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
@@ -14777,8 +14777,8 @@
       <c r="G15" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="H15" s="45"/>
-      <c r="I15" s="48"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
@@ -14790,8 +14790,8 @@
       <c r="G16" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H16" s="45"/>
-      <c r="I16" s="48"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="42"/>
     </row>
     <row r="17" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
@@ -14803,8 +14803,8 @@
       <c r="G17" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="H17" s="45"/>
-      <c r="I17" s="48"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="42"/>
     </row>
     <row r="18" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
@@ -14816,8 +14816,8 @@
       <c r="G18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="45"/>
-      <c r="I18" s="48"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="42"/>
     </row>
     <row r="19" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
@@ -14829,8 +14829,8 @@
       <c r="G19" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="H19" s="45"/>
-      <c r="I19" s="48"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="42"/>
     </row>
     <row r="20" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
@@ -14842,8 +14842,8 @@
       <c r="G20" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="H20" s="45"/>
-      <c r="I20" s="48"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="42"/>
     </row>
     <row r="21" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
@@ -14855,8 +14855,8 @@
       <c r="G21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="45"/>
-      <c r="I21" s="48"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="42"/>
     </row>
     <row r="22" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
@@ -14868,8 +14868,8 @@
       <c r="G22" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="H22" s="45"/>
-      <c r="I22" s="48"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="42"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A13">
@@ -14920,13 +14920,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="46" t="s">
         <v>111</v>
       </c>
       <c r="D2" s="28" t="s">
@@ -14934,37 +14934,37 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="28" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="28" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="28" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="43" t="s">
         <v>117</v>
       </c>
       <c r="D6" s="12" t="s">
@@ -14972,25 +14972,25 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="12" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="28" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="28" t="s">
         <v>115</v>
       </c>
@@ -15087,13 +15087,13 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="43" t="s">
         <v>135</v>
       </c>
       <c r="D17" s="12" t="s">
@@ -15101,33 +15101,33 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="12" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="12" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="12" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
       <c r="D21" s="28" t="s">
         <v>115</v>
       </c>
@@ -15297,6 +15297,101 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15664,102 +15759,44 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15782,43 +15819,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
fix bugs from AB#471
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bill.batten\Documents\Projects\STS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C62889-C1DF-4FBA-86E1-B5BB5986D4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B26C45E-B565-4CC3-AF7D-5B09C13032E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="200">
   <si>
     <t>Subsidy Control (SC) Number</t>
   </si>
@@ -1631,8 +1631,8 @@
     <col min="1" max="1" width="50.21875" style="21" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="93" style="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.21875" style="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="142.88671875" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.109375" style="21" customWidth="1"/>
+    <col min="5" max="5" width="143" style="21" customWidth="1"/>
     <col min="6" max="6" width="93" style="21" customWidth="1"/>
     <col min="7" max="7" width="42.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="61" style="19" bestFit="1" customWidth="1"/>
@@ -1664,10 +1664,10 @@
         <v>179</v>
       </c>
       <c r="D1" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>195</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>166</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>167</v>
@@ -14025,13 +14025,13 @@
           <x14:formula1>
             <xm:f>Dropdown!$H$2:$H$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E837</xm:sqref>
+          <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FB79C6B2-F23B-497C-9182-650C99B07639}">
           <x14:formula1>
             <xm:f>Dropdown!$I$2:$I$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D1048576</xm:sqref>
+          <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14043,7 +14043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -14121,33 +14123,35 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="81.599999999999994" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="142.80000000000001" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:8" ht="81.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27" t="s">
+      <c r="B6" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="142.80000000000001" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>171</v>
-      </c>
+      <c r="D6" s="27"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>

</xml_diff>

<commit_message>
updated the dropdown options for organisation size
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bill.batten\Documents\Projects\STS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B26C45E-B565-4CC3-AF7D-5B09C13032E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8120AC2D-F1A4-4384-8726-D51D18E8C14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14220" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="199">
   <si>
     <t>Subsidy Control (SC) Number</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Charity Number</t>
-  </si>
-  <si>
-    <t>Micro (fewer than 10 employees)</t>
   </si>
   <si>
     <t>Services</t>
@@ -291,9 +288,6 @@
     <t>East of England</t>
   </si>
   <si>
-    <t>Small (between 10 and 49 employees)</t>
-  </si>
-  <si>
     <t>Equity</t>
   </si>
   <si>
@@ -307,9 +301,6 @@
   </si>
   <si>
     <t>VAT Number</t>
-  </si>
-  <si>
-    <t>Medium (between 50 and 249 employees)</t>
   </si>
   <si>
     <t>Guarantee</t>
@@ -803,9 +794,6 @@
     <t>The selected file must be smaller than 500kb</t>
   </si>
   <si>
-    <t>Large (250 or more employees)</t>
-  </si>
-  <si>
     <t>Rescue subsidy</t>
   </si>
   <si>
@@ -972,6 +960,15 @@
   </si>
   <si>
     <t>Neither</t>
+  </si>
+  <si>
+    <t>SME</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>Not specified</t>
   </si>
 </sst>
 </file>
@@ -1661,22 +1658,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="37" t="s">
         <v>179</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>183</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>2</v>
@@ -1685,10 +1682,10 @@
         <v>3</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="M1" s="18" t="s">
         <v>6</v>
@@ -1709,7 +1706,7 @@
         <v>11</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="T1" s="18" t="s">
         <v>13</v>
@@ -13997,12 +13994,6 @@
           </x14:formula1>
           <xm:sqref>O2:O836</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
-          <x14:formula1>
-            <xm:f>Dropdown!$C$2:$C$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>R2:R838</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>Dropdown!$E$2:$E$4</xm:f>
@@ -14033,6 +14024,12 @@
           </x14:formula1>
           <xm:sqref>E1:E1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AD92A45A-B33A-41FA-9322-3816BFE88D9B}">
+          <x14:formula1>
+            <xm:f>Dropdown!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>R1:R1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -14057,16 +14054,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>34</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -14075,16 +14072,16 @@
     </row>
     <row r="2" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A2" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="C2" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="D2" s="27" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>38</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -14096,10 +14093,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" s="27"/>
       <c r="E3" s="2"/>
@@ -14109,14 +14106,14 @@
     </row>
     <row r="4" spans="1:8" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="27" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -14125,16 +14122,16 @@
     </row>
     <row r="5" spans="1:8" ht="142.80000000000001" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -14143,13 +14140,13 @@
     </row>
     <row r="6" spans="1:8" ht="81.599999999999994" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B6" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="27" t="s">
         <v>192</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>196</v>
       </c>
       <c r="D6" s="27"/>
       <c r="E6" s="2"/>
@@ -14159,14 +14156,14 @@
     </row>
     <row r="7" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A7" s="27" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B7" s="27"/>
       <c r="C7" s="27" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -14175,16 +14172,16 @@
     </row>
     <row r="8" spans="1:8" ht="82.2" x14ac:dyDescent="0.3">
       <c r="A8" s="27" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -14193,16 +14190,16 @@
     </row>
     <row r="9" spans="1:8" ht="305.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="C9" s="27" t="s">
         <v>189</v>
       </c>
-      <c r="B9" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>193</v>
-      </c>
       <c r="D9" s="27" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -14214,10 +14211,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D10" s="27"/>
       <c r="E10" s="2"/>
@@ -14231,7 +14228,7 @@
       </c>
       <c r="B11" s="27"/>
       <c r="C11" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="27"/>
       <c r="E11" s="2"/>
@@ -14241,13 +14238,13 @@
     </row>
     <row r="12" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="27" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="27"/>
       <c r="E12" s="2"/>
@@ -14257,11 +14254,11 @@
     </row>
     <row r="13" spans="1:8" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="27" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D13" s="27"/>
       <c r="E13" s="2"/>
@@ -14274,13 +14271,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="27" t="s">
         <v>42</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>43</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -14289,13 +14286,13 @@
     </row>
     <row r="15" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="C15" s="27" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>46</v>
       </c>
       <c r="D15" s="27"/>
       <c r="E15" s="2"/>
@@ -14308,10 +14305,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="27"/>
       <c r="E16" s="2"/>
@@ -14324,10 +14321,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="2"/>
@@ -14340,10 +14337,10 @@
         <v>10</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" s="27"/>
       <c r="E18" s="2"/>
@@ -14356,13 +14353,13 @@
         <v>11</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -14371,13 +14368,13 @@
     </row>
     <row r="20" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="27" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D20" s="27"/>
       <c r="E20" s="2"/>
@@ -14390,13 +14387,13 @@
         <v>13</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="27" t="s">
         <v>50</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>51</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -14405,16 +14402,16 @@
     </row>
     <row r="22" spans="1:8" ht="296.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="27" t="s">
         <v>52</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>164</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>53</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -14426,22 +14423,22 @@
         <v>15</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="27"/>
     </row>
     <row r="24" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="28" t="s">
         <v>55</v>
-      </c>
-      <c r="B24" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>56</v>
       </c>
       <c r="D24" s="28"/>
     </row>
@@ -14458,14 +14455,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="78.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.33203125" style="3" bestFit="1" customWidth="1"/>
@@ -14483,16 +14480,16 @@
         <v>15</v>
       </c>
       <c r="B1" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="D1" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="32" t="s">
-        <v>59</v>
-      </c>
       <c r="E1" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F1" s="32" t="s">
         <v>2</v>
@@ -14501,259 +14498,257 @@
         <v>16</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="I1" s="32" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="F2" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="H2" s="38" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>68</v>
-      </c>
       <c r="H3" s="38" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="I3" s="33" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="42" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="E4" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="G4" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="38"/>
       <c r="I4" s="33" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>160</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H5" s="38"/>
       <c r="I5" s="40"/>
     </row>
     <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="34"/>
       <c r="D6" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H6" s="38"/>
       <c r="I6" s="41"/>
     </row>
     <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H7" s="38"/>
       <c r="I7" s="42"/>
     </row>
     <row r="8" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
         <v>17</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H8" s="38"/>
       <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H9" s="38"/>
       <c r="I9" s="42"/>
     </row>
     <row r="10" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H10" s="39"/>
       <c r="I10" s="42"/>
     </row>
     <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="I11" s="42"/>
     </row>
     <row r="12" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H12" s="39"/>
       <c r="I12" s="42"/>
     </row>
     <row r="13" spans="1:9" ht="21" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H13" s="39"/>
       <c r="I13" s="42"/>
@@ -14766,7 +14761,7 @@
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H14" s="39"/>
       <c r="I14" s="42"/>
@@ -14779,7 +14774,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="H15" s="39"/>
       <c r="I15" s="42"/>
@@ -14792,7 +14787,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H16" s="39"/>
       <c r="I16" s="42"/>
@@ -14805,7 +14800,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H17" s="39"/>
       <c r="I17" s="42"/>
@@ -14818,7 +14813,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H18" s="39"/>
       <c r="I18" s="42"/>
@@ -14831,7 +14826,7 @@
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H19" s="39"/>
       <c r="I19" s="42"/>
@@ -14844,7 +14839,7 @@
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H20" s="39"/>
       <c r="I20" s="42"/>
@@ -14857,7 +14852,7 @@
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H21" s="39"/>
       <c r="I21" s="42"/>
@@ -14870,7 +14865,7 @@
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H22" s="39"/>
       <c r="I22" s="42"/>
@@ -14911,30 +14906,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14942,7 +14937,7 @@
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
       <c r="D3" s="28" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14950,7 +14945,7 @@
       <c r="B4" s="47"/>
       <c r="C4" s="47"/>
       <c r="D4" s="28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -14958,7 +14953,7 @@
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -14966,13 +14961,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -14980,7 +14975,7 @@
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
       <c r="D7" s="12" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -14988,7 +14983,7 @@
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
       <c r="D8" s="28" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -14996,7 +14991,7 @@
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="245.4" x14ac:dyDescent="0.3">
@@ -15004,11 +14999,11 @@
         <v>2</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.4">
@@ -15016,13 +15011,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="15"/>
     </row>
@@ -15031,11 +15026,11 @@
         <v>4</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="28" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -15044,10 +15039,10 @@
       </c>
       <c r="B13" s="29"/>
       <c r="C13" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>122</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="123" x14ac:dyDescent="0.3">
@@ -15055,27 +15050,27 @@
         <v>6</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="129" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -15083,11 +15078,11 @@
         <v>8</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -15095,13 +15090,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="43" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C17" s="43" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -15109,7 +15104,7 @@
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
       <c r="D18" s="12" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -15117,7 +15112,7 @@
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
       <c r="D19" s="12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -15125,7 +15120,7 @@
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
       <c r="D20" s="12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -15133,7 +15128,7 @@
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
       <c r="D21" s="28" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -15141,25 +15136,25 @@
         <v>10</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="117" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="236.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -15167,13 +15162,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="154.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -15181,23 +15176,23 @@
         <v>13</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="27" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="29" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.3">
@@ -15205,28 +15200,28 @@
         <v>15</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C27" s="28"/>
       <c r="D27" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="400.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="12" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="42" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B29" s="16"/>
       <c r="C29" s="17"/>
@@ -15234,7 +15229,7 @@
     </row>
     <row r="30" spans="1:4" ht="61.2" x14ac:dyDescent="0.3">
       <c r="A30" s="14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="17"/>
@@ -15242,7 +15237,7 @@
     </row>
     <row r="31" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" s="14" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B31" s="16"/>
       <c r="C31" s="17"/>
@@ -15250,7 +15245,7 @@
     </row>
     <row r="32" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A32" s="14" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="17"/>
@@ -15258,7 +15253,7 @@
     </row>
     <row r="33" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B33" s="16"/>
       <c r="C33" s="17"/>
@@ -15266,7 +15261,7 @@
     </row>
     <row r="34" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="17"/>
@@ -15274,7 +15269,7 @@
     </row>
     <row r="35" spans="1:4" ht="40.799999999999997" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B35" s="16"/>
       <c r="C35" s="17"/>
@@ -15301,101 +15296,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15763,44 +15663,102 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15823,6 +15781,43 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
fix: fixed misc bugs involving session variables and updated template
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan.Humphreys\Documents\BEIS STS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B52267D-71CA-4FB8-8FB5-79DBCE2D9F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA302304-8ED2-4D53-B562-B8284B98B3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1620,7 +1620,7 @@
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
@@ -13958,7 +13958,7 @@
   </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Dropdown!$E$2:$E$12</xm:f>
@@ -13988,12 +13988,6 @@
             <xm:f>Dropdown!$D$2:$D$4</xm:f>
           </x14:formula1>
           <xm:sqref>V2:V835</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000008000000}">
-          <x14:formula1>
-            <xm:f>Dropdown!$E$2:$E$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2:J835</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E0952469-FEE6-48C2-A15D-910C0C2B113B}">
           <x14:formula1>
@@ -15253,6 +15247,101 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15620,102 +15709,44 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15738,43 +15769,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
removal test data from bulk templae and updated help document
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bill.batten\Documents\Projects\STS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A1FC4A-C72C-4C0E-906E-006848C94C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0676387E-F8F7-4FDE-9189-22572AAD018B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="202">
   <si>
     <t>Subsidy Control (SC) Number</t>
   </si>
@@ -1302,6 +1302,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1319,9 +1322,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1688,7 +1688,7 @@
       <c r="I1" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="42" t="s">
         <v>200</v>
       </c>
       <c r="K1" s="17" t="s">
@@ -1762,9 +1762,7 @@
       <c r="V2" s="21"/>
       <c r="W2" s="7"/>
       <c r="X2" s="6"/>
-      <c r="Y2" s="22" t="s">
-        <v>26</v>
-      </c>
+      <c r="Y2" s="22"/>
     </row>
     <row r="3" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19"/>
@@ -14906,13 +14904,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="46" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="26" t="s">
@@ -14920,37 +14918,37 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="26" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="26" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
+      <c r="A5" s="48"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="26" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="43" t="s">
         <v>100</v>
       </c>
       <c r="D6" s="11" t="s">
@@ -14958,25 +14956,25 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="26" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="26" t="s">
         <v>98</v>
       </c>
@@ -15073,13 +15071,13 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="42" t="s">
+      <c r="C17" s="43" t="s">
         <v>118</v>
       </c>
       <c r="D17" s="11" t="s">
@@ -15087,33 +15085,33 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="43"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="11" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="11" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="11" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="44"/>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
       <c r="D21" s="26" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
feat: replace "National" with "UK-wide"
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\BEIS\source\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309513AD-9B35-4D8E-80EA-E7C2B5661B74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A780671A-DC14-4573-98E3-4329F4FBF742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="2616" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -912,29 +912,6 @@
     <t>Limit 1500 characters</t>
   </si>
   <si>
-    <t>This is the region(s) where the subsidised economic activity takes place. 
-Allowed values:
-• National
-• UK-Wide
-• GB-Wide
-• England
-• Northern Ireland
-• Scotland
-• Wales
-• East Midlands
-• East of England
-• London
-• North East
-• North West
-• South East
-• South West
-• West Midlands
-• Yorkshire and Humber</t>
-  </si>
-  <si>
-    <t>Comma separated list of one or more regions. If "National", no other regions can be included.</t>
-  </si>
-  <si>
     <t>Spending Region(s)</t>
   </si>
   <si>
@@ -1002,6 +979,28 @@
       </rPr>
       <t>This is only saved to the database if the award is standalone.</t>
     </r>
+  </si>
+  <si>
+    <t>Comma separated list of one or more regions. If "UK-wide", no other regions can be included.</t>
+  </si>
+  <si>
+    <t>This is the region(s) where the subsidised economic activity takes place. 
+Allowed values:
+• UK-wide
+• GB-wide
+• England
+• Northern Ireland
+• Scotland
+• Wales
+• East Midlands
+• East of England
+• London
+• North East
+• North West
+• South East
+• South West
+• West Midlands
+• Yorkshire and Humber</t>
   </si>
 </sst>
 </file>
@@ -1713,13 +1712,13 @@
         <v>163</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M1" s="17" t="s">
         <v>164</v>
@@ -1755,7 +1754,7 @@
         <v>14</v>
       </c>
       <c r="X1" s="17" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="Y1" s="5" t="s">
         <v>16</v>
@@ -14168,7 +14167,7 @@
         <v>172</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="2"/>
@@ -14184,7 +14183,7 @@
         <v>187</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>188</v>
@@ -14250,13 +14249,13 @@
     </row>
     <row r="11" spans="1:8" ht="88.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>151</v>
@@ -14268,16 +14267,16 @@
     </row>
     <row r="12" spans="1:8" ht="200" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -14286,14 +14285,14 @@
     </row>
     <row r="13" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="26" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -14480,16 +14479,16 @@
     </row>
     <row r="25" spans="1:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -15305,51 +15304,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -15397,6 +15351,51 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15768,6 +15767,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
@@ -15784,22 +15799,6 @@
     <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update wording in template and help docs
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\BEIS\source\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A780671A-DC14-4573-98E3-4329F4FBF742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556FA189-531E-4CAF-A66A-79CBC1CF5582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="2616" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -165,17 +165,6 @@
   </si>
   <si>
     <t>Mandatory when a Tax Measure</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1- 60000
-60001-500000
-500001-1000000
-500001-1000000
-1000001-2000000
-2000001-5000000
-5000001-10000000
-10000001-30000000
-30000001   &gt;</t>
   </si>
   <si>
     <t>Subsidy Element Full Amount Exact</t>
@@ -775,9 +764,6 @@
 </t>
   </si>
   <si>
-    <t>Where the Full Amount is a Tax Measure enter as a Range in the format shown on the next column. Two numbers seperated by a ' - '.</t>
-  </si>
-  <si>
     <t>Public Authority Name</t>
   </si>
   <si>
@@ -1001,6 +987,26 @@
 • South West
 • West Midlands
 • Yorkshire and Humber</t>
+  </si>
+  <si>
+    <t>Where the Full Amount is a Tax Measure enter as a Range in the format shown on the next column. Two numbers seperated by a ' - '. Allowed values:
+£0 to £100,000
+£100,001 to £300,000
+£300,001 to £500,000
+£500,001 to £750,000
+£750,001 to £1,500,000
+£1,500,001 to £3,000,000
+£3,000,001 to £5,000,000
+£5,000,001 to £7,500,000
+£7,500,001 to £10,000,000
+£10,000,001 to £20,000,000
+and so on in ascending ranges of £10,000,000</t>
+  </si>
+  <si>
+    <t>e.g.,
+0-100000
+100001-300000
+300001-500000…</t>
   </si>
 </sst>
 </file>
@@ -1691,40 +1697,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D1" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>147</v>
-      </c>
       <c r="H1" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="L1" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="M1" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="N1" s="17" t="s">
         <v>163</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="L1" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="N1" s="17" t="s">
-        <v>165</v>
       </c>
       <c r="O1" s="17" t="s">
         <v>6</v>
@@ -1745,7 +1751,7 @@
         <v>11</v>
       </c>
       <c r="U1" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="V1" s="17" t="s">
         <v>13</v>
@@ -1754,7 +1760,7 @@
         <v>14</v>
       </c>
       <c r="X1" s="17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="Y1" s="5" t="s">
         <v>16</v>
@@ -14127,14 +14133,14 @@
     </row>
     <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.35">
       <c r="A4" s="25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -14143,16 +14149,16 @@
     </row>
     <row r="5" spans="1:8" ht="140" x14ac:dyDescent="0.35">
       <c r="A5" s="25" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -14161,13 +14167,13 @@
     </row>
     <row r="6" spans="1:8" ht="100" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="2"/>
@@ -14177,16 +14183,16 @@
     </row>
     <row r="7" spans="1:8" ht="100" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>186</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>199</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>188</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -14195,16 +14201,16 @@
     </row>
     <row r="8" spans="1:8" ht="40" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -14213,16 +14219,16 @@
     </row>
     <row r="9" spans="1:8" ht="80" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B9" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>174</v>
-      </c>
       <c r="D9" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -14231,16 +14237,16 @@
     </row>
     <row r="10" spans="1:8" ht="305.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>169</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>171</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -14249,16 +14255,16 @@
     </row>
     <row r="11" spans="1:8" ht="88.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -14267,16 +14273,16 @@
     </row>
     <row r="12" spans="1:8" ht="200" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -14285,14 +14291,14 @@
     </row>
     <row r="13" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B13" s="25"/>
       <c r="C13" s="26" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -14301,7 +14307,7 @@
     </row>
     <row r="14" spans="1:8" ht="180" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>33</v>
@@ -14317,11 +14323,11 @@
     </row>
     <row r="15" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="2"/>
@@ -14329,7 +14335,7 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="260" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>6</v>
       </c>
@@ -14337,10 +14343,10 @@
         <v>39</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>154</v>
+        <v>200</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>40</v>
+        <v>201</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -14349,13 +14355,13 @@
     </row>
     <row r="17" spans="1:8" ht="135.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="C17" s="25" t="s">
         <v>42</v>
-      </c>
-      <c r="C17" s="25" t="s">
-        <v>43</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="2"/>
@@ -14371,7 +14377,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="2"/>
@@ -14387,7 +14393,7 @@
         <v>33</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="2"/>
@@ -14403,7 +14409,7 @@
         <v>33</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="2"/>
@@ -14419,10 +14425,10 @@
         <v>33</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -14431,13 +14437,13 @@
     </row>
     <row r="22" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D22" s="25"/>
       <c r="E22" s="2"/>
@@ -14453,10 +14459,10 @@
         <v>33</v>
       </c>
       <c r="C23" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="25" t="s">
         <v>46</v>
-      </c>
-      <c r="D23" s="25" t="s">
-        <v>47</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -14465,41 +14471,41 @@
     </row>
     <row r="24" spans="1:8" ht="80" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A26" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="26"/>
     </row>
@@ -14536,16 +14542,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="20" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="C1" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>54</v>
-      </c>
       <c r="D1" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="30" t="s">
         <v>2</v>
@@ -14554,36 +14560,36 @@
         <v>16</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>25</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -14591,54 +14597,54 @@
         <v>19</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>60</v>
-      </c>
       <c r="G3" s="36" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H3" s="31" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="42" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>62</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>63</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="36"/>
       <c r="H4" s="31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
@@ -14649,7 +14655,7 @@
         <v>22</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G5" s="36"/>
       <c r="H5" s="38"/>
@@ -14658,14 +14664,14 @@
       <c r="A6" s="9"/>
       <c r="B6" s="32"/>
       <c r="C6" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>68</v>
       </c>
       <c r="G6" s="36"/>
       <c r="H6" s="39"/>
@@ -14674,14 +14680,14 @@
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G7" s="36"/>
       <c r="H7" s="40"/>
@@ -14690,14 +14696,14 @@
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G8" s="36"/>
       <c r="H8" s="40"/>
@@ -14710,10 +14716,10 @@
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G9" s="36"/>
       <c r="H9" s="40"/>
@@ -14724,10 +14730,10 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>74</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>75</v>
       </c>
       <c r="G10" s="37"/>
       <c r="H10" s="40"/>
@@ -14738,10 +14744,10 @@
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>76</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>77</v>
       </c>
       <c r="H11" s="40"/>
     </row>
@@ -14751,10 +14757,10 @@
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="G12" s="37"/>
       <c r="H12" s="40"/>
@@ -14765,10 +14771,10 @@
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="40"/>
@@ -14780,7 +14786,7 @@
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G14" s="37"/>
       <c r="H14" s="40"/>
@@ -14792,7 +14798,7 @@
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G15" s="37"/>
       <c r="H15" s="40"/>
@@ -14804,7 +14810,7 @@
       <c r="D16" s="9"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G16" s="37"/>
       <c r="H16" s="40"/>
@@ -14816,7 +14822,7 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G17" s="37"/>
       <c r="H17" s="40"/>
@@ -14840,7 +14846,7 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19" s="37"/>
       <c r="H19" s="40"/>
@@ -14852,7 +14858,7 @@
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G20" s="37"/>
       <c r="H20" s="40"/>
@@ -14876,7 +14882,7 @@
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G22" s="37"/>
       <c r="H22" s="40"/>
@@ -14914,16 +14920,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -14931,13 +14937,13 @@
         <v>32</v>
       </c>
       <c r="B2" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="D2" s="26" t="s">
         <v>94</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14945,7 +14951,7 @@
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
       <c r="D3" s="26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14953,7 +14959,7 @@
       <c r="B4" s="47"/>
       <c r="C4" s="47"/>
       <c r="D4" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -14961,7 +14967,7 @@
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
       <c r="D5" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -14969,13 +14975,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="D6" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14983,7 +14989,7 @@
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
       <c r="D7" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14991,7 +14997,7 @@
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
       <c r="D8" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -14999,7 +15005,7 @@
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
       <c r="D9" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="240" x14ac:dyDescent="0.35">
@@ -15007,11 +15013,11 @@
         <v>2</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.45">
@@ -15019,10 +15025,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="26" t="s">
         <v>104</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>105</v>
       </c>
       <c r="D11" s="26" t="s">
         <v>37</v>
@@ -15034,11 +15040,11 @@
         <v>4</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="80.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -15047,10 +15053,10 @@
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="100" x14ac:dyDescent="0.35">
@@ -15058,27 +15064,27 @@
         <v>6</v>
       </c>
       <c r="B14" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="D14" s="25" t="s">
         <v>110</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="129" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="C15" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>113</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -15086,11 +15092,11 @@
         <v>8</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -15098,13 +15104,13 @@
         <v>9</v>
       </c>
       <c r="B17" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="D17" s="11" t="s">
         <v>118</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -15112,7 +15118,7 @@
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
       <c r="D18" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -15120,7 +15126,7 @@
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
       <c r="D19" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -15128,7 +15134,7 @@
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
       <c r="D20" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="78.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -15136,7 +15142,7 @@
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
       <c r="D21" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -15144,25 +15150,25 @@
         <v>10</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="117" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="27" t="s">
         <v>126</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>127</v>
       </c>
       <c r="C23" s="26"/>
       <c r="D23" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="236.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -15170,13 +15176,13 @@
         <v>12</v>
       </c>
       <c r="B24" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="26" t="s">
         <v>128</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -15184,23 +15190,23 @@
         <v>13</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C25" s="26"/>
       <c r="D25" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="90.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="27" t="s">
         <v>132</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>133</v>
       </c>
       <c r="C26" s="26"/>
       <c r="D26" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="288" customHeight="1" x14ac:dyDescent="0.35">
@@ -15208,28 +15214,28 @@
         <v>15</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="26"/>
       <c r="D27" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="400" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C28" s="29"/>
       <c r="D28" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="20" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="16"/>
@@ -15237,7 +15243,7 @@
     </row>
     <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="16"/>
@@ -15245,7 +15251,7 @@
     </row>
     <row r="31" spans="1:4" ht="20" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="16"/>
@@ -15253,7 +15259,7 @@
     </row>
     <row r="32" spans="1:4" ht="40" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="16"/>
@@ -15261,7 +15267,7 @@
     </row>
     <row r="33" spans="1:4" ht="40" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="16"/>
@@ -15269,7 +15275,7 @@
     </row>
     <row r="34" spans="1:4" ht="40" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="16"/>
@@ -15277,7 +15283,7 @@
     </row>
     <row r="35" spans="1:4" ht="40" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B35" s="15"/>
       <c r="C35" s="16"/>
@@ -15304,6 +15310,51 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -15351,51 +15402,6 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15767,22 +15773,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
@@ -15799,6 +15789,22 @@
     <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
AB# update bulk upload help text and validation
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hajra.hassan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.robinson\Documents\BEIS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F3A2F7-C7E1-437B-8306-5FD2A16D0101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496B9F0E-2804-4454-A84C-B9BCD4463531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="204">
   <si>
     <t>Subsidy Control (SC) Number</t>
   </si>
@@ -892,9 +892,6 @@
     <t>Specific policy objective</t>
   </si>
   <si>
-    <t>Mandatory, when award is standalone</t>
-  </si>
-  <si>
     <t>Limit 1500 characters</t>
   </si>
   <si>
@@ -939,21 +936,6 @@
 Subsidies or Schemes of Interest (SSoI)
 Subsidies or Schemes of Particular Interest (SSoPI)
 Neither
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>This is only saved to the database if the award is standalone.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Specific Policy Objective(s) - provide details of the policy objective(s) of the scheme or subsidy. This should reflect the specific policy objective(s) documented under Subsidy Control Principle A (which forms part of Step 1 of the Assessment Framework in the Statutory Guidance for the UK Subsidy Control Regime).
 </t>
     </r>
     <r>
@@ -1016,6 +998,98 @@
   </si>
   <si>
     <t>Limit 5000 characters</t>
+  </si>
+  <si>
+    <r>
+      <t>Specific Policy Objective(s) - provide details of the policy objective(s) of the scheme or subsidy. This should reflect the specific policy objective(s) documented under Subsidy Control Principle A (which forms part of Step 1 of the Assessment Framework in the Statutory Guidance for the UK Subsidy Control Regime).
+This field is</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> only saved and published</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>standalone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> awards. If you are submitting an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>in-scheme</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> award, the information entered here will </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>not be recorded</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.
+Please include the policy objective in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Subsidy Description</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> field (Field G) instead.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1728,16 +1802,16 @@
         <v>161</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>162</v>
@@ -1773,7 +1847,7 @@
         <v>14</v>
       </c>
       <c r="Y1" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z1" s="5" t="s">
         <v>16</v>
@@ -14092,8 +14166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A4" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14198,7 +14272,7 @@
         <v>170</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="2"/>
@@ -14206,18 +14280,18 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="102.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>184</v>
       </c>
       <c r="B7" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>185</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>186</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -14280,16 +14354,16 @@
     </row>
     <row r="11" spans="1:8" ht="305.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -14298,13 +14372,13 @@
     </row>
     <row r="12" spans="1:8" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>150</v>
@@ -14316,16 +14390,16 @@
     </row>
     <row r="13" spans="1:8" ht="204" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>189</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>190</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -14334,14 +14408,14 @@
     </row>
     <row r="14" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>192</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>193</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -14386,10 +14460,10 @@
         <v>39</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -14528,16 +14602,16 @@
     </row>
     <row r="26" spans="1:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B26" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
@@ -15353,101 +15427,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15815,44 +15794,102 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15875,6 +15912,43 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
checkout latest version of bulk upload template from CR0006
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hajra.hassan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.robinson\Documents\BEIS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F3A2F7-C7E1-437B-8306-5FD2A16D0101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496B9F0E-2804-4454-A84C-B9BCD4463531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="204">
   <si>
     <t>Subsidy Control (SC) Number</t>
   </si>
@@ -892,9 +892,6 @@
     <t>Specific policy objective</t>
   </si>
   <si>
-    <t>Mandatory, when award is standalone</t>
-  </si>
-  <si>
     <t>Limit 1500 characters</t>
   </si>
   <si>
@@ -939,21 +936,6 @@
 Subsidies or Schemes of Interest (SSoI)
 Subsidies or Schemes of Particular Interest (SSoPI)
 Neither
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>This is only saved to the database if the award is standalone.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Specific Policy Objective(s) - provide details of the policy objective(s) of the scheme or subsidy. This should reflect the specific policy objective(s) documented under Subsidy Control Principle A (which forms part of Step 1 of the Assessment Framework in the Statutory Guidance for the UK Subsidy Control Regime).
 </t>
     </r>
     <r>
@@ -1016,6 +998,98 @@
   </si>
   <si>
     <t>Limit 5000 characters</t>
+  </si>
+  <si>
+    <r>
+      <t>Specific Policy Objective(s) - provide details of the policy objective(s) of the scheme or subsidy. This should reflect the specific policy objective(s) documented under Subsidy Control Principle A (which forms part of Step 1 of the Assessment Framework in the Statutory Guidance for the UK Subsidy Control Regime).
+This field is</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> only saved and published</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>standalone</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> awards. If you are submitting an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>in-scheme</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> award, the information entered here will </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>not be recorded</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.
+Please include the policy objective in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Subsidy Description</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> field (Field G) instead.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1728,16 +1802,16 @@
         <v>161</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L1" s="17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N1" s="17" t="s">
         <v>162</v>
@@ -1773,7 +1847,7 @@
         <v>14</v>
       </c>
       <c r="Y1" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="Z1" s="5" t="s">
         <v>16</v>
@@ -14092,8 +14166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A4" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14198,7 +14272,7 @@
         <v>170</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="2"/>
@@ -14206,18 +14280,18 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="102.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A7" s="25" t="s">
         <v>184</v>
       </c>
       <c r="B7" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="25" t="s">
         <v>185</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>197</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>186</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -14280,16 +14354,16 @@
     </row>
     <row r="11" spans="1:8" ht="305.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="25" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -14298,13 +14372,13 @@
     </row>
     <row r="12" spans="1:8" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>150</v>
@@ -14316,16 +14390,16 @@
     </row>
     <row r="13" spans="1:8" ht="204" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>189</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>190</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -14334,14 +14408,14 @@
     </row>
     <row r="14" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="26" t="s">
+        <v>191</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>192</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>193</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -14386,10 +14460,10 @@
         <v>39</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -14528,16 +14602,16 @@
     </row>
     <row r="26" spans="1:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B26" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
@@ -15353,101 +15427,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15815,44 +15794,102 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15875,6 +15912,43 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
AB#143 granting date to confirmation date
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adam.robinson\Documents\BEIS\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496B9F0E-2804-4454-A84C-B9BCD4463531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852C8F67-6970-486A-85D7-4CA7FEA8B1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="205">
   <si>
     <t>Subsidy Control (SC) Number</t>
   </si>
@@ -1090,6 +1090,9 @@
       </rPr>
       <t xml:space="preserve"> field (Field G) instead.</t>
     </r>
+  </si>
+  <si>
+    <t>Award confirmation Date</t>
   </si>
 </sst>
 </file>
@@ -1767,7 +1770,7 @@
     <col min="20" max="20" width="53.44140625" style="19" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="50.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="80.21875" style="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="33.44140625" style="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="39.21875" style="19" customWidth="1"/>
     <col min="24" max="24" width="37" style="19" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="90.6640625" style="19" customWidth="1"/>
     <col min="26" max="26" width="108.6640625" style="19" bestFit="1" customWidth="1"/>
@@ -1841,7 +1844,7 @@
         <v>153</v>
       </c>
       <c r="W1" s="17" t="s">
-        <v>13</v>
+        <v>204</v>
       </c>
       <c r="X1" s="17" t="s">
         <v>14</v>
@@ -15427,6 +15430,101 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15794,102 +15892,44 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15912,43 +15952,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
updated bulk upload template
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgigbr-my.sharepoint.com/personal/leah_cooney_cgi_com/Documents/sts/transparency-db-admin-portal/public/assets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{11DB9AAE-4209-495F-A552-B582A987C672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FA8BC61-105A-4DD5-B12E-9A4DC29FBE6E}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{11DB9AAE-4209-495F-A552-B582A987C672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E5F1235-9944-472D-881B-5F14A1B79E86}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="208">
   <si>
     <t>Subsidy Control (SC) Number</t>
   </si>
@@ -895,9 +895,6 @@
     <t>Limit 1500 characters</t>
   </si>
   <si>
-    <t>Spending Region(s)</t>
-  </si>
-  <si>
     <t>Subsidy Purpose</t>
   </si>
   <si>
@@ -947,28 +944,6 @@
       </rPr>
       <t>This is only saved to the database if the award is standalone.</t>
     </r>
-  </si>
-  <si>
-    <t>Comma separated list of one or more regions. If "UK-wide", no other regions can be included.</t>
-  </si>
-  <si>
-    <t>This is the region(s) where the subsidised economic activity takes place. 
-Allowed values:
-• UK-wide
-• GB-wide
-• England
-• Northern Ireland
-• Scotland
-• Wales
-• East Midlands
-• East of England
-• London
-• North East
-• North West
-• South East
-• South West
-• West Midlands
-• Yorkshire and Humber</t>
   </si>
   <si>
     <t>Where the Full Amount is a Tax Measure enter as a Range in the format shown on the next column. Two numbers seperated by a ' - '. Allowed values:
@@ -1117,6 +1092,28 @@
   </si>
   <si>
     <t>Geographical Location(s)</t>
+  </si>
+  <si>
+    <t>This is the geographical location(s) where the subsidised economic activity takes place. 
+Allowed values:
+• UK-wide
+• GB-wide
+• England
+• Northern Ireland
+• Scotland
+• Wales
+• East Midlands
+• East of England
+• London
+• North East
+• North West
+• South East
+• South West
+• West Midlands
+• Yorkshire and Humber</t>
+  </si>
+  <si>
+    <t>Comma separated list of one or more geographical location. If "UK-wide", no other geographical locations can be included.</t>
   </si>
 </sst>
 </file>
@@ -1500,6 +1497,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1765,10 +1766,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Z29" sqref="Z29"/>
-      <selection pane="bottomLeft" activeCell="Z1" sqref="Z1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.3"/>
@@ -1814,7 +1815,7 @@
         <v>145</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>173</v>
@@ -1832,16 +1833,16 @@
         <v>161</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="L1" s="42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M1" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O1" s="17" t="s">
         <v>162</v>
@@ -1871,13 +1872,13 @@
         <v>153</v>
       </c>
       <c r="X1" s="17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="Y1" s="17" t="s">
         <v>14</v>
       </c>
       <c r="Z1" s="17" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AA1" s="5" t="s">
         <v>16</v>
@@ -14206,7 +14207,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView zoomScale="54" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -14304,13 +14307,13 @@
     </row>
     <row r="6" spans="1:8" ht="61.8" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>169</v>
@@ -14328,7 +14331,7 @@
         <v>170</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="2"/>
@@ -14344,7 +14347,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>185</v>
@@ -14410,16 +14413,16 @@
     </row>
     <row r="12" spans="1:8" ht="305.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -14428,13 +14431,13 @@
     </row>
     <row r="13" spans="1:8" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>150</v>
@@ -14446,16 +14449,16 @@
     </row>
     <row r="14" spans="1:8" ht="204" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>188</v>
-      </c>
-      <c r="D14" s="25" t="s">
-        <v>189</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -14464,14 +14467,14 @@
     </row>
     <row r="15" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>191</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>192</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -14516,10 +14519,10 @@
         <v>39</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -14658,16 +14661,16 @@
     </row>
     <row r="27" spans="1:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="D27" s="25" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
@@ -15483,51 +15486,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
-    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
-    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
-    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Value>1</Value>
-    </TaxCatchAll>
-    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Invision>
-    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
-        </TermInfo>
-      </Terms>
-    </m975189f4ba442ecbf67d4147307b177>
-    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
-    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
-    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
-    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
-      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
-      <Description>E67A7M7FTMSZ-519618591-1208</Description>
-    </_dlc_DocIdUrl>
-    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15895,6 +15853,51 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
+    <Date_x0020_Opened xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">2020-09-02T20:32:49+00:00</Date_x0020_Opened>
+    <LegacyData xmlns="aaacb922-5235-4a66-b188-303b9b46fbd7" xsi:nil="true"/>
+    <Descriptor xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Value>1</Value>
+    </TaxCatchAll>
+    <Invision xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Invision>
+    <m975189f4ba442ecbf67d4147307b177 xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">BEIS:Corporate Services:Digital Directorate:EU Exit, BRM and Assurance:EBRASS</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">10b60d33-9f3b-419c-b326-e542b5592571</TermId>
+        </TermInfo>
+      </Terms>
+    </m975189f4ba442ecbf67d4147307b177>
+    <Security_x0020_Classification xmlns="0063f72e-ace3-48fb-9c1f-5b513408b31f">OFFICIAL</Security_x0020_Classification>
+    <ijmz xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+    <Retention_x0020_Label xmlns="a8f60570-4bd3-4f2b-950b-a996de8ab151" xsi:nil="true"/>
+    <Date_x0020_Closed xmlns="b413c3fd-5a3b-4239-b985-69032e371c04" xsi:nil="true"/>
+    <_dlc_DocId xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">E67A7M7FTMSZ-519618591-1208</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="4ff8cd83-fc61-4182-af0d-9444b096b4cc">
+      <Url>https://beisgov.sharepoint.com/sites/SCPTDbase/_layouts/15/DocIdRedir.aspx?ID=E67A7M7FTMSZ-519618591-1208</Url>
+      <Description>E67A7M7FTMSZ-519618591-1208</Description>
+    </_dlc_DocIdUrl>
+    <Invisiondesigns xmlns="58eecf05-07e6-460c-a17a-1e6913e0d7ae" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
@@ -15946,9 +15949,24 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
+    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
+    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
+    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
+    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
+    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15975,24 +15993,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
-    <ds:schemaRef ds:uri="0063f72e-ace3-48fb-9c1f-5b513408b31f"/>
-    <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
-    <ds:schemaRef ds:uri="a8f60570-4bd3-4f2b-950b-a996de8ab151"/>
-    <ds:schemaRef ds:uri="aaacb922-5235-4a66-b188-303b9b46fbd7"/>
-    <ds:schemaRef ds:uri="58eecf05-07e6-460c-a17a-1e6913e0d7ae"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Update mandatory test for SC number and Scheme Title
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\BEIS\source\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EF0F57-F3FB-483A-8868-8188BAF7FA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F31BDA-7AFE-40EF-B814-839DC31D328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="210">
   <si>
     <t>Subsidy Control (SC) Number</t>
   </si>
@@ -1114,6 +1114,12 @@
   </si>
   <si>
     <t>Comma separated list of one or more geographical location. If "UK-wide", no other geographical locations can be included.</t>
+  </si>
+  <si>
+    <t>Mandatory if subsidy scheme title is not entered</t>
+  </si>
+  <si>
+    <t>Mandatory if subsidy control number is not entered</t>
   </si>
 </sst>
 </file>
@@ -14203,7 +14209,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView zoomScale="54" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14231,12 +14239,12 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="40" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>33</v>
+        <v>208</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>34</v>
@@ -14249,12 +14257,12 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="40" x14ac:dyDescent="0.35">
       <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>33</v>
+        <v>209</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>36</v>
@@ -15480,15 +15488,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Government_x0020_Body xmlns="b413c3fd-5a3b-4239-b985-69032e371c04">BEIS</Government_x0020_Body>
@@ -15524,7 +15523,66 @@
 </p:properties>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15892,65 +15950,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="b413c3fd-5a3b-4239-b985-69032e371c04"/>
@@ -15971,7 +15971,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15994,14 +16010,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>

<commit_message>
Update specific policy objective wording in help doc. Move legal basis up the table in help document. Fix a couple of typos in help doc and template.
</commit_message>
<xml_diff>
--- a/public/assets/files/Bulk_Upload_Awards_template.xlsx
+++ b/public/assets/files/Bulk_Upload_Awards_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\BEIS\source\transparency-db-admin-portal\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F31BDA-7AFE-40EF-B814-839DC31D328A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E8F5003-FC3D-43DE-80E5-B31BE82D2F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="2616" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Upload Template" sheetId="1" r:id="rId1"/>
@@ -944,20 +944,6 @@
       </rPr>
       <t>This is only saved to the database if the award is standalone.</t>
     </r>
-  </si>
-  <si>
-    <t>Where the Full Amount is a Tax Measure enter as a Range in the format shown on the next column. Two numbers seperated by a ' - '. Allowed values:
-£0 to £100,000
-£100,001 to £300,000
-£300,001 to £500,000
-£500,001 to £750,000
-£750,001 to £1,500,000
-£1,500,001 to £3,000,000
-£3,000,001 to £5,000,000
-£5,000,001 to £7,500,000
-£7,500,001 to £10,000,000
-£10,000,001 to £20,000,000
-and so on in ascending ranges of £10,000,000</t>
   </si>
   <si>
     <t>e.g.,
@@ -1120,6 +1106,20 @@
   </si>
   <si>
     <t>Mandatory if subsidy control number is not entered</t>
+  </si>
+  <si>
+    <t>Where the Full Amount is a Tax Measure enter as a Range in the format shown on the next column. Two numbers separated by a ' - '. Allowed values:
+£0 to £100,000
+£100,001 to £300,000
+£300,001 to £500,000
+£500,001 to £750,000
+£750,001 to £1,500,000
+£1,500,001 to £3,000,000
+£3,000,001 to £5,000,000
+£5,000,001 to £7,500,000
+£7,500,001 to £10,000,000
+£10,000,001 to £20,000,000
+and so on in ascending ranges of £10,000,000</t>
   </si>
 </sst>
 </file>
@@ -1817,7 +1817,7 @@
         <v>145</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F1" s="17" t="s">
         <v>173</v>
@@ -1829,7 +1829,7 @@
         <v>146</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J1" s="34" t="s">
         <v>160</v>
@@ -1874,13 +1874,13 @@
         <v>153</v>
       </c>
       <c r="X1" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="Y1" s="17" t="s">
         <v>14</v>
       </c>
       <c r="Z1" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AA1" s="5" t="s">
         <v>16</v>
@@ -14209,8 +14209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A16" zoomScale="54" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14244,7 +14244,7 @@
         <v>32</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>34</v>
@@ -14262,7 +14262,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>36</v>
@@ -14309,13 +14309,13 @@
     </row>
     <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.35">
       <c r="A6" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="C6" s="25" t="s">
         <v>203</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>204</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>169</v>
@@ -14349,7 +14349,7 @@
         <v>33</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>185</v>
@@ -14379,16 +14379,16 @@
     </row>
     <row r="10" spans="1:8" ht="305.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C10" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>198</v>
-      </c>
-      <c r="D10" s="25" t="s">
-        <v>199</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -14521,10 +14521,10 @@
         <v>39</v>
       </c>
       <c r="C18" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>195</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>196</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -14663,16 +14663,16 @@
     </row>
     <row r="27" spans="1:8" ht="409.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="D27" s="25" t="s">
         <v>206</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -15524,65 +15524,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010095552673811A1544B9DC17E80367E3D9" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c219bbdc66874a295362540fe1f1ca4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4ff8cd83-fc61-4182-af0d-9444b096b4cc" xmlns:ns3="0063f72e-ace3-48fb-9c1f-5b513408b31f" xmlns:ns4="b413c3fd-5a3b-4239-b985-69032e371c04" xmlns:ns5="a8f60570-4bd3-4f2b-950b-a996de8ab151" xmlns:ns6="aaacb922-5235-4a66-b188-303b9b46fbd7" xmlns:ns7="58eecf05-07e6-460c-a17a-1e6913e0d7ae" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ea492d8f6df3c516113149b290687b47" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="" ns7:_="">
     <xsd:import namespace="4ff8cd83-fc61-4182-af0d-9444b096b4cc"/>
@@ -15950,6 +15891,65 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FBEDEBF5-0F8B-43D7-9E7F-E4CDAE2C086C}">
   <ds:schemaRefs>
@@ -15972,22 +15972,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB723818-A5CD-443A-A314-BAC9891A4BF8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16010,6 +15994,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AF44877-6D21-41C2-9736-04B57D725022}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6216EEDE-1870-4B1D-BF90-D3816A946FAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{d9290083-bd2f-48a2-8ac5-09a524b17d15}" enabled="1" method="Privileged" siteId="{b9fec68c-c92d-461e-9a97-3d03a0f18b82}" contentBits="1" removed="0"/>

</xml_diff>